<commit_message>
corrected first year calendar error
</commit_message>
<xml_diff>
--- a/data/excel_files/FormattedJun2023.xlsx
+++ b/data/excel_files/FormattedJun2023.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -49,7 +49,7 @@
     <t>BreakFast</t>
   </si>
   <si>
-    <t>Acad</t>
+    <t>Vacation</t>
   </si>
   <si>
     <t>Lunch</t>
@@ -59,9 +59,6 @@
   </si>
   <si>
     <t>Dinner</t>
-  </si>
-  <si>
-    <t>Vacation</t>
   </si>
 </sst>
 </file>
@@ -1368,7 +1365,7 @@
         <v>0.0</v>
       </c>
       <c r="H38" s="1">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="39">
@@ -1395,7 +1392,7 @@
         <v>0.0</v>
       </c>
       <c r="H39" s="1">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="40">
@@ -1422,7 +1419,7 @@
         <v>0.0</v>
       </c>
       <c r="H40" s="1">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="41">
@@ -1449,7 +1446,7 @@
         <v>0.0</v>
       </c>
       <c r="H41" s="1">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="42">
@@ -1476,7 +1473,7 @@
         <v>0.0</v>
       </c>
       <c r="H42" s="1">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="43">
@@ -1503,7 +1500,7 @@
         <v>0.0</v>
       </c>
       <c r="H43" s="1">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="44">
@@ -1530,7 +1527,7 @@
         <v>0.0</v>
       </c>
       <c r="H44" s="1">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="45">
@@ -1557,7 +1554,7 @@
         <v>0.0</v>
       </c>
       <c r="H45" s="1">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="46">
@@ -1584,7 +1581,7 @@
         <v>0.0</v>
       </c>
       <c r="H46" s="1">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="47">
@@ -1611,7 +1608,7 @@
         <v>0.0</v>
       </c>
       <c r="H47" s="1">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="48">
@@ -1638,7 +1635,7 @@
         <v>0.0</v>
       </c>
       <c r="H48" s="1">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="49">
@@ -1665,7 +1662,7 @@
         <v>0.0</v>
       </c>
       <c r="H49" s="1">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="50">
@@ -1692,7 +1689,7 @@
         <v>0.0</v>
       </c>
       <c r="H50" s="1">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="51">
@@ -1719,7 +1716,7 @@
         <v>0.0</v>
       </c>
       <c r="H51" s="1">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="52">
@@ -1746,7 +1743,7 @@
         <v>0.0</v>
       </c>
       <c r="H52" s="1">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="53">
@@ -1773,7 +1770,7 @@
         <v>0.0</v>
       </c>
       <c r="H53" s="1">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="54">
@@ -1800,7 +1797,7 @@
         <v>0.0</v>
       </c>
       <c r="H54" s="1">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="55">
@@ -1827,7 +1824,7 @@
         <v>0.0</v>
       </c>
       <c r="H55" s="1">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="56">
@@ -1848,7 +1845,7 @@
         <v>0.0</v>
       </c>
       <c r="H56" s="1">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="57">
@@ -1875,7 +1872,7 @@
         <v>0.0</v>
       </c>
       <c r="H57" s="1">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="58">
@@ -2100,7 +2097,7 @@
         <v>32.0</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F66" s="1">
         <v>4.0</v>
@@ -2127,7 +2124,7 @@
         <v>46.0</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F67" s="1">
         <v>4.0</v>
@@ -2154,7 +2151,7 @@
         <v>17.0</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F68" s="1">
         <v>4.0</v>
@@ -2181,7 +2178,7 @@
         <v>25.0</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F69" s="1">
         <v>4.0</v>
@@ -2205,7 +2202,7 @@
         <v>17.0</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F70" s="1">
         <v>4.0</v>
@@ -2232,7 +2229,7 @@
         <v>30.0</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F71" s="1">
         <v>4.0</v>
@@ -2253,7 +2250,7 @@
         <v>14</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F72" s="1">
         <v>4.0</v>
@@ -2280,7 +2277,7 @@
         <v>35.0</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F73" s="1">
         <v>4.0</v>
@@ -2307,7 +2304,7 @@
         <v>30.0</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F74" s="1">
         <v>0.0</v>
@@ -2334,7 +2331,7 @@
         <v>36.0</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F75" s="1">
         <v>0.0</v>
@@ -2361,7 +2358,7 @@
         <v>18.0</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F76" s="1">
         <v>0.0</v>
@@ -2388,7 +2385,7 @@
         <v>42.0</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F77" s="1">
         <v>0.0</v>
@@ -2415,7 +2412,7 @@
         <v>33.0</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F78" s="1">
         <v>0.0</v>
@@ -2442,7 +2439,7 @@
         <v>43.0</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F79" s="1">
         <v>0.0</v>
@@ -2466,7 +2463,7 @@
         <v>3.0</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F80" s="1">
         <v>0.0</v>
@@ -2490,7 +2487,7 @@
         <v>28.0</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F81" s="1">
         <v>0.0</v>
@@ -2517,7 +2514,7 @@
         <v>40.0</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F82" s="1">
         <v>0.0</v>
@@ -2544,7 +2541,7 @@
         <v>48.0</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F83" s="1">
         <v>0.0</v>
@@ -2571,7 +2568,7 @@
         <v>13.0</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F84" s="1">
         <v>0.0</v>
@@ -2598,7 +2595,7 @@
         <v>51.0</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F85" s="1">
         <v>0.0</v>
@@ -2625,7 +2622,7 @@
         <v>27.0</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F86" s="1">
         <v>0.0</v>
@@ -2652,7 +2649,7 @@
         <v>35.0</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F87" s="1">
         <v>0.0</v>
@@ -2676,7 +2673,7 @@
         <v>7.0</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F88" s="1">
         <v>0.0</v>
@@ -2700,7 +2697,7 @@
         <v>30.0</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F89" s="1">
         <v>0.0</v>
@@ -2727,7 +2724,7 @@
         <v>40.0</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F90" s="1">
         <v>0.0</v>
@@ -2754,7 +2751,7 @@
         <v>33.0</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F91" s="1">
         <v>0.0</v>
@@ -2781,7 +2778,7 @@
         <v>16.0</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F92" s="1">
         <v>0.0</v>
@@ -2808,7 +2805,7 @@
         <v>40.0</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F93" s="1">
         <v>0.0</v>
@@ -2835,7 +2832,7 @@
         <v>31.0</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F94" s="1">
         <v>1.0</v>
@@ -2859,7 +2856,7 @@
         <v>99.0</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F95" s="1">
         <v>1.0</v>
@@ -2880,7 +2877,7 @@
         <v>14</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F96" s="1">
         <v>1.0</v>
@@ -2907,7 +2904,7 @@
         <v>30.0</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F97" s="1">
         <v>1.0</v>
@@ -2934,7 +2931,7 @@
         <v>68.0</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F98" s="1">
         <v>1.0</v>
@@ -2961,7 +2958,7 @@
         <v>24.0</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F99" s="1">
         <v>1.0</v>
@@ -2988,7 +2985,7 @@
         <v>30.0</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F100" s="1">
         <v>1.0</v>
@@ -3015,7 +3012,7 @@
         <v>47.0</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F101" s="1">
         <v>1.0</v>
@@ -3042,7 +3039,7 @@
         <v>34.0</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F102" s="1">
         <v>0.0</v>
@@ -3069,7 +3066,7 @@
         <v>37.0</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F103" s="1">
         <v>0.0</v>
@@ -3090,7 +3087,7 @@
         <v>14</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F104" s="1">
         <v>0.0</v>
@@ -3114,7 +3111,7 @@
         <v>69.0</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F105" s="1">
         <v>0.0</v>
@@ -3141,7 +3138,7 @@
         <v>28.0</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F106" s="1">
         <v>0.0</v>
@@ -3168,7 +3165,7 @@
         <v>36.0</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F107" s="1">
         <v>0.0</v>
@@ -3189,7 +3186,7 @@
         <v>14</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F108" s="1">
         <v>0.0</v>
@@ -3213,7 +3210,7 @@
         <v>43.0</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F109" s="1">
         <v>0.0</v>
@@ -3240,7 +3237,7 @@
         <v>38.0</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F110" s="1">
         <v>0.0</v>
@@ -3267,7 +3264,7 @@
         <v>37.0</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F111" s="1">
         <v>0.0</v>
@@ -3294,7 +3291,7 @@
         <v>22.0</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F112" s="1">
         <v>0.0</v>
@@ -3321,7 +3318,7 @@
         <v>50.0</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F113" s="1">
         <v>0.0</v>
@@ -3348,7 +3345,7 @@
         <v>20.0</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F114" s="1">
         <v>0.0</v>
@@ -3375,7 +3372,7 @@
         <v>32.0</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F115" s="1">
         <v>0.0</v>
@@ -3399,7 +3396,7 @@
         <v>4.0</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F116" s="1">
         <v>0.0</v>
@@ -3423,7 +3420,7 @@
         <v>52.0</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F117" s="1">
         <v>0.0</v>
@@ -3450,7 +3447,7 @@
         <v>24.0</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F118" s="1">
         <v>0.0</v>
@@ -3477,7 +3474,7 @@
         <v>27.0</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F119" s="1">
         <v>0.0</v>
@@ -3501,7 +3498,7 @@
         <v>2.0</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F120" s="1">
         <v>0.0</v>
@@ -3528,7 +3525,7 @@
         <v>30.0</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F121" s="1">
         <v>0.0</v>

</xml_diff>